<commit_message>
Updating the Base_Map_Closed to the 2019.2 PreScan Version
</commit_message>
<xml_diff>
--- a/AD-EYE/Experiments/Base_Map_Closed/Simulation/TAconstant.xlsx
+++ b/AD-EYE/Experiments/Base_Map_Closed/Simulation/TAconstant.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Base_Map\Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Base_Map_Closed\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E7816-5DA8-41C2-816E-CD9C28540635}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06F3059-6AB5-4624-883B-B9ED295EF820}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>